<commit_message>
tried pushing whatsapp files on render
</commit_message>
<xml_diff>
--- a/QuizResults.xlsx
+++ b/QuizResults.xlsx
@@ -397,7 +397,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E8"/>
+  <dimension ref="A1:E23"/>
   <sheetViews>
     <sheetView workbookViewId="0" rightToLeft="0"/>
   </sheetViews>
@@ -538,9 +538,264 @@
         <v>4b0631dc</v>
       </c>
     </row>
+    <row r="9">
+      <c r="A9" t="str">
+        <v>Yashshree</v>
+      </c>
+      <c r="B9">
+        <v>2</v>
+      </c>
+      <c r="C9" t="str">
+        <v>chinmaymhatre21@gmail.com</v>
+      </c>
+      <c r="D9" t="str">
+        <v>19/11/2024, 6:41:05 pm</v>
+      </c>
+      <c r="E9" t="str">
+        <v>34734b0c</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="str">
+        <v>Khushil</v>
+      </c>
+      <c r="B10">
+        <v>2</v>
+      </c>
+      <c r="C10" t="str">
+        <v>khushilbhimani2@gmail.com</v>
+      </c>
+      <c r="D10" t="str">
+        <v>19/11/2024, 6:53:00 pm</v>
+      </c>
+      <c r="E10" t="str">
+        <v>c881e563</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="str">
+        <v>Khushil</v>
+      </c>
+      <c r="B11">
+        <v>2</v>
+      </c>
+      <c r="C11" t="str">
+        <v>khushilbhimani2@gmail.com</v>
+      </c>
+      <c r="D11" t="str">
+        <v>19/11/2024, 7:01:01 pm</v>
+      </c>
+      <c r="E11" t="str">
+        <v>80a40d9e</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="str">
+        <v>Khushil</v>
+      </c>
+      <c r="B12">
+        <v>2</v>
+      </c>
+      <c r="C12" t="str">
+        <v>khushilbhimani2@gmail.com</v>
+      </c>
+      <c r="D12" t="str">
+        <v>19/11/2024, 7:04:46 pm</v>
+      </c>
+      <c r="E12" t="str">
+        <v>122441d0</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="str">
+        <v>Khushil Girish Bhimani</v>
+      </c>
+      <c r="B13">
+        <v>2</v>
+      </c>
+      <c r="C13" t="str">
+        <v>khushilbhimani302@gmail.com</v>
+      </c>
+      <c r="D13" t="str">
+        <v>19/11/2024, 7:06:07 pm</v>
+      </c>
+      <c r="E13" t="str">
+        <v>ecb8c446</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="str">
+        <v>Khushil Bhimani</v>
+      </c>
+      <c r="B14">
+        <v>2</v>
+      </c>
+      <c r="C14" t="str">
+        <v>khushilbhimani2@gmail.com</v>
+      </c>
+      <c r="D14" t="str">
+        <v>19/11/2024, 7:13:09 pm</v>
+      </c>
+      <c r="E14" t="str">
+        <v>555e4dae</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="str">
+        <v>Khush</v>
+      </c>
+      <c r="B15">
+        <v>2</v>
+      </c>
+      <c r="C15" t="str">
+        <v>khushilbhimani2@gmail.com</v>
+      </c>
+      <c r="D15" t="str">
+        <v>19/11/2024, 7:14:38 pm</v>
+      </c>
+      <c r="E15" t="str">
+        <v>19c59d21</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="str">
+        <v>Khushil</v>
+      </c>
+      <c r="B16">
+        <v>2</v>
+      </c>
+      <c r="C16" t="str">
+        <v>Khushilbhimani2@gmail.com</v>
+      </c>
+      <c r="D16" t="str">
+        <v>19/11/2024, 7:16:28 pm</v>
+      </c>
+      <c r="E16" t="str">
+        <v>c9e25a3c</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="str">
+        <v>Khushil Bhimani</v>
+      </c>
+      <c r="B17">
+        <v>2</v>
+      </c>
+      <c r="C17" t="str">
+        <v>khushilbhimani302@gmail.com</v>
+      </c>
+      <c r="D17" t="str">
+        <v>19/11/2024, 7:19:07 pm</v>
+      </c>
+      <c r="E17" t="str">
+        <v>6cd1327d</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="str">
+        <v>Khuhsil</v>
+      </c>
+      <c r="B18">
+        <v>2</v>
+      </c>
+      <c r="C18" t="str">
+        <v>Khushilbhimani302@gmail.com</v>
+      </c>
+      <c r="D18" t="str">
+        <v>19/11/2024, 7:20:14 pm</v>
+      </c>
+      <c r="E18" t="str">
+        <v>7ab50f23</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="str">
+        <v>Khushil Girish Bhimani</v>
+      </c>
+      <c r="B19">
+        <v>2</v>
+      </c>
+      <c r="C19" t="str">
+        <v>khushilbhimani302@gmail.com</v>
+      </c>
+      <c r="D19" t="str">
+        <v>19/11/2024, 7:21:18 pm</v>
+      </c>
+      <c r="E19" t="str">
+        <v>4e6b9388</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="str">
+        <v>pradipgarhwal183@gmail.com</v>
+      </c>
+      <c r="B20">
+        <v>2</v>
+      </c>
+      <c r="C20" t="str">
+        <v>pradipgarhwal183@gmail.com</v>
+      </c>
+      <c r="D20" t="str">
+        <v>19/11/2024, 7:40:59 pm</v>
+      </c>
+      <c r="E20" t="str">
+        <v>0dbacf79</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="str">
+        <v>Chinmay Mhatre</v>
+      </c>
+      <c r="B21">
+        <v>2</v>
+      </c>
+      <c r="C21" t="str">
+        <v>chinmaymhatre21@gmail.com</v>
+      </c>
+      <c r="D21" t="str">
+        <v>21/11/2024, 12:28:26 am</v>
+      </c>
+      <c r="E21" t="str">
+        <v>9878e1fd</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="str">
+        <v>Pradip Garhwal</v>
+      </c>
+      <c r="B22">
+        <v>2</v>
+      </c>
+      <c r="C22" t="str">
+        <v>pradipgarhwal183@gmail.com</v>
+      </c>
+      <c r="D22" t="str">
+        <v>21/11/2024, 12:30:20 am</v>
+      </c>
+      <c r="E22" t="str">
+        <v>99e18d11</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="str">
+        <v>Rohit Gautam</v>
+      </c>
+      <c r="B23">
+        <v>0</v>
+      </c>
+      <c r="C23" t="str">
+        <v>rohit@hacktify.in</v>
+      </c>
+      <c r="D23" t="str">
+        <v>21/11/2024, 12:44:09 am</v>
+      </c>
+      <c r="E23" t="str">
+        <v>2a846fa0</v>
+      </c>
+    </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:E8"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:E23"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
added quiz without payment
</commit_message>
<xml_diff>
--- a/QuizResults.xlsx
+++ b/QuizResults.xlsx
@@ -397,7 +397,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E23"/>
+  <dimension ref="A1:E29"/>
   <sheetViews>
     <sheetView workbookViewId="0" rightToLeft="0"/>
   </sheetViews>
@@ -793,9 +793,111 @@
         <v>2a846fa0</v>
       </c>
     </row>
+    <row r="24">
+      <c r="A24" t="str">
+        <v>Chinmay Mhatre</v>
+      </c>
+      <c r="B24">
+        <v>2</v>
+      </c>
+      <c r="C24" t="str">
+        <v>chinmayrmhatre@gmail.com</v>
+      </c>
+      <c r="D24" t="str">
+        <v>13/12/2024, 4:10:39 pm</v>
+      </c>
+      <c r="E24" t="str">
+        <v>05779eb0</v>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="str">
+        <v>Chinmay Mhatre</v>
+      </c>
+      <c r="B25">
+        <v>2</v>
+      </c>
+      <c r="C25" t="str">
+        <v>chinmayrmhatre@gmail.com</v>
+      </c>
+      <c r="D25" t="str">
+        <v>13/12/2024, 4:39:25 pm</v>
+      </c>
+      <c r="E25" t="str">
+        <v>8f08a72f</v>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="str">
+        <v>Khushil Girish Bhimani</v>
+      </c>
+      <c r="B26">
+        <v>2</v>
+      </c>
+      <c r="C26" t="str">
+        <v>Khushilbhimani2@gmail.com</v>
+      </c>
+      <c r="D26" t="str">
+        <v>15/12/2024, 7:12:05 pm</v>
+      </c>
+      <c r="E26" t="str">
+        <v>f8ab2fd2</v>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="str">
+        <v>Khushil Bhimani</v>
+      </c>
+      <c r="B27">
+        <v>2</v>
+      </c>
+      <c r="C27" t="str">
+        <v>khushilbhimani302@gmail.com</v>
+      </c>
+      <c r="D27" t="str">
+        <v>15/12/2024, 7:17:29 pm</v>
+      </c>
+      <c r="E27" t="str">
+        <v>dc89af5f</v>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="str">
+        <v>Khushil Girish Bhimani</v>
+      </c>
+      <c r="B28">
+        <v>2</v>
+      </c>
+      <c r="C28" t="str">
+        <v>khushilbhimani2@gmail.com</v>
+      </c>
+      <c r="D28" t="str">
+        <v>15/12/2024, 7:31:07 pm</v>
+      </c>
+      <c r="E28" t="str">
+        <v>24abf7bc</v>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" t="str">
+        <v>Rohit Gautam</v>
+      </c>
+      <c r="B29">
+        <v>0</v>
+      </c>
+      <c r="C29" t="str">
+        <v>rohit@hacktify.in</v>
+      </c>
+      <c r="D29" t="str">
+        <v>15/12/2024, 7:42:21 pm</v>
+      </c>
+      <c r="E29" t="str">
+        <v>b609cfb8</v>
+      </c>
+    </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:E23"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:E29"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>